<commit_message>
day 2 is done
</commit_message>
<xml_diff>
--- a/rm/Java Road Map.xlsx
+++ b/rm/Java Road Map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">SNO</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.youtube.com/playlist?list=PLv2-IhRmhbyTsIWz57SxNpMpSB_QOX9JY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docker deep dive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1MahP66iPthHOi42gqmHf84cFMNM4WVm4/view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1jWavXffzr2-0FVBGfYA3x7Rt-_m9TS9v/view?usp=sharing</t>
   </si>
   <si>
     <t xml:space="preserve">Sucess: if we follow one path...</t>
@@ -246,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,6 +298,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -418,10 +431,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -653,7 +666,7 @@
       <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="5"/>
@@ -674,9 +687,33 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2" t="s">
+    <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>36</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -687,6 +724,7 @@
     <hyperlink ref="C2" r:id="rId1" display="https://www.youtube.com/watch?v=QH18cZwDOyU&amp;list=PLv2-IhRmhbyQpigiJ-cO1rz8Plp0tzSmY&amp;index=2&amp;t=476s&amp;ab_channel=BusyCoderAcademy"/>
     <hyperlink ref="C6" r:id="rId2" display="https://drive.google.com/file/d/1H4vHj-2MgzJ-ZN2al3rKk3GrJNscufcp/view?usp=sharing"/>
     <hyperlink ref="C17" r:id="rId3" display="https://www.youtube.com/watch?v=9BAVhAbVLU4&amp;t=9172s&amp;ab_channel=BusyCoderAcademy"/>
+    <hyperlink ref="C20" r:id="rId4" display="https://drive.google.com/file/d/1jWavXffzr2-0FVBGfYA3x7Rt-_m9TS9v/view?usp=sharing"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>